<commit_message>
Adjusted Gamestate Naming to eliminate TextId
</commit_message>
<xml_diff>
--- a/src/main/resources/text_layers.xlsx
+++ b/src/main/resources/text_layers.xlsx
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DFCA99-905A-465D-82AC-724A0E1582CC}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="173" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Textboxes, text csv,pom.xml
</commit_message>
<xml_diff>
--- a/src/main/resources/text_layers.xlsx
+++ b/src/main/resources/text_layers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365-my.sharepoint.com/personal/jasmin_gyger_students_fhnw_ch/Documents/Semester/Module S2/IP2/algaecare/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{97DD4EEE-EC6D-473D-8655-D9D44CC6271C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E6AF43-ED8F-9B43-98A1-C84213785444}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{97DD4EEE-EC6D-473D-8655-D9D44CC6271C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{967BC944-5F17-A540-9418-17C770FB3327}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{145AF9C6-CCDD-403B-B7D4-3574F7C66631}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{145AF9C6-CCDD-403B-B7D4-3574F7C66631}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>FR</t>
-  </si>
-  <si>
     <t>TITLE</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
   </si>
   <si>
     <t>AXOLOTL_INTRODUCTION</t>
-  </si>
-  <si>
-    <t>EN</t>
   </si>
   <si>
     <t>NOT_OBJECT</t>
@@ -189,10 +180,6 @@
 Ich zähle auf dich, damit mein Zuhause schön bleibt!</t>
   </si>
   <si>
-    <t>Oh nein,  Müll landet leider oft im Meer! Er verschmutzt unser Wasser, blockiert das Sonnenlicht für die Algen wodurch sie absterben und ist gefährlich für alle Meerestiere. Das schadet dem ganzen Ökosystem!
-&gt; Versuche es mit einem anderen Objekt</t>
-  </si>
-  <si>
     <t>Malheureusement, ce n'était pas l'axolotl.
 Trouve le bon objet et place-le en haut de la zone lumineuse pour commencer le jeu.</t>
   </si>
@@ -305,6 +292,26 @@
   <si>
     <t>Oh no, unfortunately garbage often ends up in the sea! It pollutes our water, blocks the sunlight for the algae, causing them to die and is dangerous for all marine animals. It harms the whole ecosystem!
 &gt; Try another object</t>
+  </si>
+  <si>
+    <t>Oh nein, Müll landet leider oft im Meer! Er verschmutzt unser Wasser, blockiert das Sonnenlicht für die Algen wodurch sie absterben und ist gefährlich für alle Meerestiere. Das schadet dem ganzen Ökosystem!
+&gt; Versuche es mit einem anderen Objekt</t>
+  </si>
+  <si>
+    <t>OBJECT_TRASH_GRABBER</t>
+  </si>
+  <si>
+    <t>Stark! Mit Abfallzangen können wir Küsten und Strände sauber halten und Abfall aus dem Meer fischen. Sie helfen das Wasser sauber zu halten um Algen genug Licht und Platz zum wachsen zu geben. Das ist zwar hilfreich aber nicht die Lösung für das Problem!
+&gt; Wähle ein nächstes Objekt aus</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>en</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DFCA99-905A-465D-82AC-724A0E1582CC}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="173" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1170,273 +1177,281 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="128" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>